<commit_message>
Updated as of 10-11-2023
</commit_message>
<xml_diff>
--- a/Bijaya Samillani 2023.xlsx
+++ b/Bijaya Samillani 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{0CE8CCE8-955F-4E83-83F4-B6C744211777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CD704D-0B1A-41C8-BF5B-E73481BA8B88}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="8_{0CE8CCE8-955F-4E83-83F4-B6C744211777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8477B17C-96E0-45E6-BC3A-A562EE38F64A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{151D4641-7C4D-442B-80AA-9BD3BCEAEAFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{151D4641-7C4D-442B-80AA-9BD3BCEAEAFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Tab" sheetId="1" r:id="rId1"/>
@@ -31,80 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>sounak nandi</author>
-  </authors>
-  <commentList>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{07F631F9-F115-42CB-B7ED-A41312BB2174}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>sounak nandi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-1. 30 k advance to Caterar
-2. 14 k morning payment  caterar
-3. 1k + 5k to madhu da
-4. 31820 to caterar final</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>sounak nandi</author>
-  </authors>
-  <commentList>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{AFB6A86B-40DA-401B-A505-CB09F250AFEC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>sounak nandi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-15 - Chicken
-70 - Mutton</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="67">
   <si>
     <t>Provider</t>
   </si>
@@ -112,9 +40,6 @@
     <t>Payment mode</t>
   </si>
   <si>
-    <t>Start Caterar</t>
-  </si>
-  <si>
     <t>Type of Food</t>
   </si>
   <si>
@@ -202,111 +127,138 @@
     <t>Zaqir Da</t>
   </si>
   <si>
-    <t>1. 2 --&gt; Speaks
-2. 2 --&gt; Mics
-3. Lights for kitchn Areas
+    <t>Coupon Printing</t>
+  </si>
+  <si>
+    <t>Providers</t>
+  </si>
+  <si>
+    <t>Catering</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>Bottle Water</t>
+  </si>
+  <si>
+    <t>Decoration</t>
+  </si>
+  <si>
+    <t>Sound and Light</t>
+  </si>
+  <si>
+    <t>Payment Done</t>
+  </si>
+  <si>
+    <t>Total Budget</t>
+  </si>
+  <si>
+    <t>BIJAYA SAMILLANI 2023</t>
+  </si>
+  <si>
+    <t>Funds</t>
+  </si>
+  <si>
+    <t>CGWA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAND TOTAL </t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>Money received</t>
+  </si>
+  <si>
+    <t>Thermocol</t>
+  </si>
+  <si>
+    <t>Additional Materials</t>
+  </si>
+  <si>
+    <t>Extra Coupon</t>
+  </si>
+  <si>
+    <t>Cleaning and Tips</t>
+  </si>
+  <si>
+    <t>ALL CLEAR</t>
+  </si>
+  <si>
+    <t>Blinkit and additionals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment on </t>
+  </si>
+  <si>
+    <t>Funds From</t>
+  </si>
+  <si>
+    <t>Funds Used</t>
+  </si>
+  <si>
+    <t>Payment Initial</t>
+  </si>
+  <si>
+    <t>Payment Final</t>
+  </si>
+  <si>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>1. 2 --&gt; 15 Feet table with veils
+2. 8 --&gt; Round tables with veild
+3. Red carpets for lawn
+4. 2 --&gt; Tables for keeping water jars
+5. Stage with backdrop
+7. Tripol for Non veg and veg area kitchen
+8. Table for kitchn areas
+9. Tripol for outside food area
+10. 2 extra tables for Snacks counter
+11. Transportation
+12. Labour cost for fitting and unfitting</t>
+  </si>
+  <si>
+    <t>1. 2 --&gt; Speaker
+2. 2 --&gt; Mic
+3. Lights for kitchen Areas
 4. Lights for Exterior - Dinner area
 5. Lights for Event area
-6. One mixer with 2 boosting</t>
-  </si>
-  <si>
-    <t>Coupon Printing</t>
-  </si>
-  <si>
-    <t>Providers</t>
-  </si>
-  <si>
-    <t>Catering</t>
-  </si>
-  <si>
-    <t>Sweets</t>
-  </si>
-  <si>
-    <t>Bottle Water</t>
-  </si>
-  <si>
-    <t>Decoration</t>
-  </si>
-  <si>
-    <t>Sound and Light</t>
-  </si>
-  <si>
-    <t>Payment Done</t>
-  </si>
-  <si>
-    <t>Total Budget</t>
-  </si>
-  <si>
-    <t>BIJAYA SAMILLANI 2023</t>
-  </si>
-  <si>
-    <t>Funds</t>
-  </si>
-  <si>
-    <t>CGWA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAND TOTAL </t>
-  </si>
-  <si>
-    <t>Coupon</t>
-  </si>
-  <si>
-    <t>Money received</t>
-  </si>
-  <si>
-    <t>1. 2 --&gt; 15 Feet table with veils
-2. 8 --&gt; Round tables with veild
-3. Umbrellas for exterior
-4. Red carpets for lawn
-5. 2 --&gt; Tables for keeping water jars
-6. Stage with backdrop
-8. Tripol for Non veg and veg area kitchen
-9. Table for kitchn areas
-10. Tripol for outside food area</t>
-  </si>
-  <si>
-    <t>Thermocol</t>
-  </si>
-  <si>
-    <t>Additional Materials</t>
-  </si>
-  <si>
-    <t>Extra Coupon</t>
-  </si>
-  <si>
-    <t>Cleaning and Tips</t>
-  </si>
-  <si>
-    <t>ALL CLEAR</t>
-  </si>
-  <si>
-    <t>Blinkit and additionals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment on </t>
-  </si>
-  <si>
-    <t>Funds From</t>
-  </si>
-  <si>
-    <t>Funds Used</t>
-  </si>
-  <si>
-    <t>Payment Initial</t>
-  </si>
-  <si>
-    <t>Payment Final</t>
-  </si>
-  <si>
-    <t>Estimated</t>
+6. One mixer with 2 boosting
+7. 5 stand Fans
+8. Labur and sound man
+9. Transportation
+10. Fitting and UnFitting</t>
+  </si>
+  <si>
+    <t>Star Caterar</t>
+  </si>
+  <si>
+    <t>Final Cleaning</t>
+  </si>
+  <si>
+    <t>Advance - 1</t>
+  </si>
+  <si>
+    <t>Advance - 2</t>
+  </si>
+  <si>
+    <t>Last Payment</t>
+  </si>
+  <si>
+    <t>Returned</t>
+  </si>
+  <si>
+    <t>In Hand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,20 +280,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,8 +392,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -519,41 +473,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -711,15 +645,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -768,11 +693,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -780,24 +718,60 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -807,28 +781,49 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -840,13 +835,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -858,17 +851,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -885,118 +878,134 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1037,6 +1046,14 @@
 </file>
 
 <file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1336,11 +1353,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D335F8A-874C-4865-9DED-53F1D2E6D267}">
-  <dimension ref="E4:J29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D335F8A-874C-4865-9DED-53F1D2E6D267}">
+  <dimension ref="E4:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1349,89 +1366,105 @@
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" customWidth="1"/>
+    <col min="9" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E5" s="40"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="36"/>
-    </row>
-    <row r="6" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="41"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="37"/>
-    </row>
-    <row r="7" spans="5:10" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="41"/>
-      <c r="F7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="37"/>
-    </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E8" s="41"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="37"/>
-    </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E9" s="41"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="37"/>
-    </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E10" s="41"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="37"/>
-    </row>
-    <row r="11" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="41"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="41"/>
+    <row r="4" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E5" s="71"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="71"/>
+    </row>
+    <row r="6" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="72"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="72"/>
+    </row>
+    <row r="7" spans="5:12" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="72"/>
+      <c r="F7" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="72"/>
+    </row>
+    <row r="8" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E8" s="72"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="72"/>
+    </row>
+    <row r="9" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E9" s="72"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="72"/>
+    </row>
+    <row r="10" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E10" s="72"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="72"/>
+    </row>
+    <row r="11" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="72"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="72"/>
+    </row>
+    <row r="12" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="72"/>
       <c r="F12" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E13" s="41"/>
-      <c r="F13" s="26" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="72"/>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="72"/>
+      <c r="F13" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="G13" s="7">
         <f>Catering!H15</f>
@@ -1441,20 +1474,22 @@
         <f>Catering!H10</f>
         <v>81880</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="18">
         <f>H13-G13</f>
         <v>0</v>
       </c>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E14" s="41"/>
-      <c r="F14" s="27" t="s">
-        <v>36</v>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="72"/>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="72"/>
+      <c r="F14" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="G14" s="2">
-        <f>Sweets!H11</f>
-        <v>0</v>
+        <f>Sweets!H10</f>
+        <v>3000</v>
       </c>
       <c r="H14" s="2">
         <f>Sweets!H8</f>
@@ -1462,18 +1497,20 @@
       </c>
       <c r="I14" s="5">
         <f t="shared" ref="I14:I18" si="0">H14-G14</f>
-        <v>3000</v>
-      </c>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E15" s="41"/>
-      <c r="F15" s="27" t="s">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="72"/>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="72"/>
+      <c r="F15" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="G15" s="2">
-        <f>'Bottle Water'!H11</f>
-        <v>0</v>
+        <f>'Bottle Water'!H10</f>
+        <v>900</v>
       </c>
       <c r="H15" s="2">
         <f>'Bottle Water'!H8</f>
@@ -1481,148 +1518,177 @@
       </c>
       <c r="I15" s="5">
         <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="J15" s="37"/>
-    </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E16" s="41"/>
-      <c r="F16" s="27" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="72"/>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="72"/>
+      <c r="F16" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="G16" s="2">
         <f>Decoration!F12</f>
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="H16" s="2">
         <f>Decoration!F8</f>
-        <v>9000</v>
+        <v>10000</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E17" s="41"/>
-      <c r="F17" s="27" t="s">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="72"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E17" s="72"/>
+      <c r="F17" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="G17" s="2">
-        <f>'Sound &amp; Light'!F11</f>
-        <v>0</v>
+        <f>'Sound &amp; Light'!F10</f>
+        <v>4000</v>
       </c>
       <c r="H17" s="2">
         <f>'Sound &amp; Light'!F8</f>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="J17" s="37"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E18" s="41"/>
-      <c r="F18" s="27" t="s">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="72"/>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="72"/>
+      <c r="F18" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="G18" s="2">
-        <f>'Additional Materials'!E13</f>
-        <v>0</v>
+        <f>'Additional Materials'!E14</f>
+        <v>1260</v>
       </c>
       <c r="H18" s="2">
-        <f>'Additional Materials'!E10</f>
-        <v>662</v>
+        <f>'Additional Materials'!E11</f>
+        <v>1260</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="0"/>
-        <v>662</v>
-      </c>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E19" s="41"/>
-      <c r="F19" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="72"/>
+    </row>
+    <row r="19" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="72"/>
+      <c r="F19" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="56">
+        <f>SUM(G13:G18)</f>
+        <v>101040</v>
+      </c>
+      <c r="H19" s="56">
+        <f t="shared" ref="H19:I19" si="1">SUM(H13:H18)</f>
+        <v>101040</v>
+      </c>
+      <c r="I19" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="72"/>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E20" s="72"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="72"/>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E21" s="72"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="72"/>
+    </row>
+    <row r="22" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="72"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="72"/>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="72"/>
+      <c r="F23" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="16">
-        <f>SUM(G13:G18)</f>
-        <v>87880</v>
-      </c>
-      <c r="H19" s="16">
-        <f t="shared" ref="H19:I19" si="1">SUM(H13:H18)</f>
-        <v>98442</v>
-      </c>
-      <c r="I19" s="29">
-        <f t="shared" si="1"/>
-        <v>10562</v>
-      </c>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E20" s="41"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="37"/>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E21" s="41"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="37"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E22" s="41"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E23" s="41"/>
-      <c r="F23" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E24" s="41"/>
-      <c r="F24" s="2" t="s">
-        <v>44</v>
+      <c r="G23" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" s="72"/>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E24" s="72"/>
+      <c r="F24" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="G24" s="2">
-        <f>SUM(Catering!H23,Catering!H9,Sweets!H8,'Bottle Water'!H8,Decoration!F8,'Sound &amp; Light'!F8,'Additional Materials'!E10)</f>
-        <v>92382</v>
+        <v>100000</v>
       </c>
       <c r="H24" s="2">
-        <v>81820</v>
+        <f>SUM(Catering!H11,Catering!H12,Catering!H14,Sweets!H9,'Bottle Water'!H9,Decoration!F9,Decoration!F10,Decoration!F11,'Sound &amp; Light'!F9,'Additional Materials'!E12)</f>
+        <v>94980</v>
       </c>
       <c r="I24" s="2">
         <f>G24-H24</f>
-        <v>10562</v>
-      </c>
-      <c r="J24" s="37"/>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E25" s="41"/>
-      <c r="F25" s="2" t="s">
-        <v>46</v>
+        <v>5020</v>
+      </c>
+      <c r="J24" s="2">
+        <v>5020</v>
+      </c>
+      <c r="K24" s="53">
+        <f>I24-J24</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="72"/>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="72"/>
+      <c r="F25" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="G25" s="2">
         <f>Catering!H26</f>
@@ -1635,72 +1701,93 @@
         <f>G25-H25</f>
         <v>0</v>
       </c>
-      <c r="J25" s="37"/>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E26" s="41"/>
-      <c r="F26" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="30">
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="53">
+        <f>I25-J25</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="72"/>
+    </row>
+    <row r="26" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="72"/>
+      <c r="F26" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="61">
         <f>SUM(G24:G25)</f>
-        <v>98442</v>
-      </c>
-      <c r="H26" s="30">
+        <v>106060</v>
+      </c>
+      <c r="H26" s="61">
         <f t="shared" ref="H26:I26" si="2">SUM(H24:H25)</f>
-        <v>87880</v>
-      </c>
-      <c r="I26" s="30">
+        <v>101040</v>
+      </c>
+      <c r="I26" s="61">
         <f t="shared" si="2"/>
-        <v>10562</v>
-      </c>
-      <c r="J26" s="37"/>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E27" s="41"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="37"/>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E28" s="41"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="37"/>
-    </row>
-    <row r="29" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="42"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="38"/>
+        <v>5020</v>
+      </c>
+      <c r="J26" s="61">
+        <v>5020</v>
+      </c>
+      <c r="K26" s="61">
+        <f>I26-J26</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="72"/>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E27" s="72"/>
+      <c r="F27" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="72"/>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E28" s="72"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="72"/>
+    </row>
+    <row r="29" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E29" s="73"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F5:I6"/>
-    <mergeCell ref="J5:J29"/>
-    <mergeCell ref="F27:I29"/>
     <mergeCell ref="E5:E29"/>
     <mergeCell ref="F8:I11"/>
     <mergeCell ref="F20:I22"/>
+    <mergeCell ref="L5:L29"/>
+    <mergeCell ref="F27:K29"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F5:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F0B90-5779-4078-9D1D-1055E93B6651}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F0B90-5779-4078-9D1D-1055E93B6651}">
   <dimension ref="D6:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,27 +1803,27 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="52" t="s">
-        <v>2</v>
+      <c r="D7" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2">
         <v>360</v>
@@ -1748,12 +1835,12 @@
         <f>G7*F7</f>
         <v>24120</v>
       </c>
-      <c r="I7" s="53"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="52"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2">
         <v>660</v>
@@ -1765,23 +1852,23 @@
         <f>G8*F8</f>
         <v>56760</v>
       </c>
-      <c r="I8" s="53"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="8"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2">
         <v>1000</v>
       </c>
-      <c r="I9" s="53"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1793,14 +1880,14 @@
         <f>SUM(H7:H9)</f>
         <v>81880</v>
       </c>
-      <c r="I10" s="53"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="59" t="s">
-        <v>12</v>
+      <c r="D11" s="43" t="s">
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1808,11 +1895,11 @@
         <v>30000</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="60"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1820,11 +1907,11 @@
         <v>14000</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="60"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1832,11 +1919,11 @@
         <v>6060</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="61"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1844,12 +1931,12 @@
         <v>31820</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1861,7 +1948,7 @@
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -1870,44 +1957,44 @@
         <f>H10-H15</f>
         <v>0</v>
       </c>
-      <c r="I16" s="57" t="s">
-        <v>53</v>
+      <c r="I16" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="5:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E21" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E21" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="17">
+      <c r="F21" s="16">
         <v>360</v>
       </c>
       <c r="G21" s="7">
         <f>G7-G24</f>
         <v>63</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <f>G21*F21</f>
         <v>22680</v>
       </c>
     </row>
     <row r="22" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="65"/>
-      <c r="F22" s="18">
+      <c r="E22" s="40"/>
+      <c r="F22" s="17">
         <v>660</v>
       </c>
       <c r="G22" s="4">
@@ -1920,24 +2007,24 @@
       </c>
     </row>
     <row r="23" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="65"/>
-      <c r="F23" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="20">
+      <c r="E23" s="40"/>
+      <c r="F23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="19">
         <f>SUM(G21:G22)</f>
         <v>142</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="20">
         <f>SUM(H21:H22)</f>
         <v>74820</v>
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="17">
+      <c r="E24" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="16">
         <v>360</v>
       </c>
       <c r="G24" s="7">
@@ -1949,8 +2036,8 @@
       </c>
     </row>
     <row r="25" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="55"/>
-      <c r="F25" s="18">
+      <c r="E25" s="41"/>
+      <c r="F25" s="17">
         <v>660</v>
       </c>
       <c r="G25" s="4">
@@ -1962,50 +2049,49 @@
       </c>
     </row>
     <row r="26" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="56"/>
-      <c r="F26" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="20">
+      <c r="E26" s="42"/>
+      <c r="F26" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="19">
         <f>SUM(G24:G25)</f>
         <v>11</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="20">
         <f>SUM(H24:H25)</f>
         <v>6060</v>
       </c>
     </row>
     <row r="27" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E27" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22">
+        <v>49</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21">
         <v>1000</v>
       </c>
     </row>
     <row r="28" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25">
+      <c r="E28" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24">
         <f>SUM(H26,H23,H27)</f>
         <v>81880</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="I7:I10"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D7:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2023,10 +2109,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDF985F-91AC-43D9-8BF5-AF6764EC419F}">
-  <dimension ref="D6:I12"/>
+  <dimension ref="D6:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2042,16 +2128,16 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>1</v>
@@ -2059,10 +2145,10 @@
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2">
         <v>15</v>
@@ -2075,12 +2161,12 @@
         <v>3000</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" ht="18" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -2089,60 +2175,52 @@
         <f>SUM(H7:H7)</f>
         <v>3000</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>3000</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="54"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
+        <f>SUM(H9:H9)</f>
+        <v>3000</v>
+      </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9">
-        <f>SUM(H9:H10)</f>
+        <f>H8-H10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9">
-        <f>H8-H11</f>
-        <v>3000</v>
+      <c r="I11" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D9:D10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2151,7 +2229,7 @@
           <x14:formula1>
             <xm:f>'Payment modes'!$D$6:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>I7:I10</xm:sqref>
+          <xm:sqref>I7 I9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2161,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99B3E53-F6EE-4463-AF9F-C232C8163FF9}">
-  <dimension ref="D6:I12"/>
+  <dimension ref="D6:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,27 +2258,27 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
         <v>90</v>
@@ -2213,12 +2291,12 @@
         <v>900</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="4:9" ht="18" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -2228,59 +2306,53 @@
         <v>900</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>900</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="54"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
+        <f>SUM(H9:H9)</f>
+        <v>900</v>
+      </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9">
-        <f>SUM(H9:H10)</f>
+        <f>H8-H10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9">
-        <f>H8-H11</f>
-        <v>900</v>
+      <c r="I11" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D9:D10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2289,7 +2361,7 @@
           <x14:formula1>
             <xm:f>'Payment modes'!$D$6:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>I9 I7</xm:sqref>
+          <xm:sqref>I7 I9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2301,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFCD54E-8F6C-48C8-8EF2-F1E444066224}">
   <dimension ref="D6:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2317,90 +2389,102 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="216" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F7" s="2">
-        <v>9000</v>
-      </c>
-      <c r="G7" s="53"/>
+        <v>10000</v>
+      </c>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9">
-        <f>SUM(F7:F7)</f>
-        <v>9000</v>
-      </c>
-      <c r="G8" s="53"/>
+        <v>10000</v>
+      </c>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="D9" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" s="2">
         <v>1000</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="54"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F10" s="2">
         <v>5000</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="11"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9">
         <f>SUM(F9:F11)</f>
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9">
         <f>F8-F12</f>
-        <v>3000</v>
+        <v>0</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D9:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2410,7 +2494,7 @@
           <x14:formula1>
             <xm:f>'Payment modes'!$D$6:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G10</xm:sqref>
+          <xm:sqref>G9:G11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2420,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864B976B-F79D-43CE-B35D-AC6B45D1C19C}">
-  <dimension ref="D6:G12"/>
+  <dimension ref="D6:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,78 +2522,75 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="144" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2">
-        <v>3000</v>
-      </c>
-      <c r="G7" s="53"/>
+        <v>4000</v>
+      </c>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9">
-        <f>SUM(F7:F7)</f>
-        <v>3000</v>
-      </c>
-      <c r="G8" s="53"/>
+        <v>4000</v>
+      </c>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="54" t="s">
-        <v>12</v>
+      <c r="D9" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>4000</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="54"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9">
+        <f>SUM(F9:F9)</f>
+        <v>4000</v>
+      </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9">
-        <f>SUM(F9:F10)</f>
+        <f>F8-F10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9">
-        <f>F8-F11</f>
-        <v>3000</v>
+      <c r="G11" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2529,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977346C3-FB40-4906-BFEF-5578C3F0829E}">
-  <dimension ref="D6:F14"/>
+  <dimension ref="D6:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2543,88 +2624,103 @@
   <sheetData>
     <row r="6" spans="4:6" ht="18" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2">
         <v>120</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2">
         <v>170</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="D10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2">
+        <v>600</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="4:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="D11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9">
+        <f>SUM(E7:E10)</f>
+        <v>1260</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="9">
-        <f>SUM(E7:E9)</f>
-        <v>662</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="11"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>1260</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="9">
-        <f>SUM(E11:E11)</f>
-        <v>0</v>
-      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E14" s="9">
-        <f>E10-E13</f>
-        <v>662</v>
+        <f>SUM(E12:E12)</f>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="9">
+        <f>E11-E14</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2636,7 +2732,7 @@
           <x14:formula1>
             <xm:f>'Payment modes'!$D$6:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F7:F9 F11:F12</xm:sqref>
+          <xm:sqref>F7:F10 F12:F13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2648,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA0FD11-AEA6-48EE-ACA9-F949F47C87AE}">
   <dimension ref="D5:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" activeCellId="1" sqref="A12:XFD12 A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2659,37 +2755,37 @@
   <sheetData>
     <row r="5" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes as of 17-11-2023
</commit_message>
<xml_diff>
--- a/Bijaya Samillani 2023.xlsx
+++ b/Bijaya Samillani 2023.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="179" documentId="8_{0CE8CCE8-955F-4E83-83F4-B6C744211777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8477B17C-96E0-45E6-BC3A-A562EE38F64A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{151D4641-7C4D-442B-80AA-9BD3BCEAEAFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{151D4641-7C4D-442B-80AA-9BD3BCEAEAFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Tab" sheetId="1" r:id="rId1"/>
@@ -851,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -894,79 +894,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -974,30 +905,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1007,6 +914,96 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1372,79 +1369,79 @@
   <sheetData>
     <row r="4" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E5" s="71"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="71"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="40"/>
     </row>
     <row r="6" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="72"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="72"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="5:12" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="72"/>
-      <c r="F7" s="68" t="s">
+      <c r="E7" s="41"/>
+      <c r="F7" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="72"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="41"/>
     </row>
     <row r="8" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E8" s="72"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="72"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="41"/>
     </row>
     <row r="9" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E9" s="72"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="72"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="41"/>
     </row>
     <row r="10" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E10" s="72"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="72"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="72"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="72"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="41"/>
     </row>
     <row r="12" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="72"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="13" t="s">
         <v>32</v>
       </c>
@@ -1457,12 +1454,12 @@
       <c r="I12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="72"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="41"/>
     </row>
     <row r="13" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E13" s="72"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="25" t="s">
         <v>33</v>
       </c>
@@ -1478,12 +1475,12 @@
         <f>H13-G13</f>
         <v>0</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="72"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E14" s="72"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="26" t="s">
         <v>34</v>
       </c>
@@ -1499,12 +1496,12 @@
         <f t="shared" ref="I14:I18" si="0">H14-G14</f>
         <v>0</v>
       </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="72"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="72"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="26" t="s">
         <v>35</v>
       </c>
@@ -1520,12 +1517,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="72"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="41"/>
     </row>
     <row r="16" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E16" s="72"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="26" t="s">
         <v>36</v>
       </c>
@@ -1541,12 +1538,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="72"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E17" s="72"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="26" t="s">
         <v>37</v>
       </c>
@@ -1562,12 +1559,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="72"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="41"/>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E18" s="72"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="26" t="s">
         <v>47</v>
       </c>
@@ -1583,85 +1580,85 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="72"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="72"/>
-      <c r="F19" s="55" t="s">
+      <c r="E19" s="41"/>
+      <c r="F19" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="56">
+      <c r="G19" s="33">
         <f>SUM(G13:G18)</f>
         <v>101040</v>
       </c>
-      <c r="H19" s="56">
+      <c r="H19" s="33">
         <f t="shared" ref="H19:I19" si="1">SUM(H13:H18)</f>
         <v>101040</v>
       </c>
-      <c r="I19" s="57">
+      <c r="I19" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="72"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="41"/>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E20" s="72"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="72"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="41"/>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E21" s="72"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="72"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="41"/>
     </row>
     <row r="22" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="72"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="72"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E23" s="72"/>
-      <c r="F23" s="58" t="s">
+      <c r="E23" s="41"/>
+      <c r="F23" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="I23" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="59" t="s">
+      <c r="J23" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="70" t="s">
+      <c r="K23" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="L23" s="72"/>
+      <c r="L23" s="41"/>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E24" s="72"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="26" t="s">
         <v>42</v>
       </c>
@@ -1679,14 +1676,14 @@
       <c r="J24" s="2">
         <v>5020</v>
       </c>
-      <c r="K24" s="53">
+      <c r="K24" s="31">
         <f>I24-J24</f>
         <v>0</v>
       </c>
-      <c r="L24" s="72"/>
+      <c r="L24" s="41"/>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E25" s="72"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="26" t="s">
         <v>44</v>
       </c>
@@ -1704,69 +1701,69 @@
       <c r="J25" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="53">
+      <c r="K25" s="31">
         <f>I25-J25</f>
         <v>0</v>
       </c>
-      <c r="L25" s="72"/>
+      <c r="L25" s="41"/>
     </row>
     <row r="26" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="72"/>
-      <c r="F26" s="60" t="s">
+      <c r="E26" s="41"/>
+      <c r="F26" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="61">
+      <c r="G26" s="38">
         <f>SUM(G24:G25)</f>
         <v>106060</v>
       </c>
-      <c r="H26" s="61">
+      <c r="H26" s="38">
         <f t="shared" ref="H26:I26" si="2">SUM(H24:H25)</f>
         <v>101040</v>
       </c>
-      <c r="I26" s="61">
+      <c r="I26" s="38">
         <f t="shared" si="2"/>
         <v>5020</v>
       </c>
-      <c r="J26" s="61">
+      <c r="J26" s="38">
         <v>5020</v>
       </c>
-      <c r="K26" s="61">
+      <c r="K26" s="38">
         <f>I26-J26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="72"/>
+      <c r="L26" s="41"/>
     </row>
     <row r="27" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E27" s="72"/>
-      <c r="F27" s="62" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="72"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="41"/>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E28" s="72"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="72"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="41"/>
     </row>
     <row r="29" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="73"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="73"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1786,7 +1783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F0B90-5779-4078-9D1D-1055E93B6651}">
   <dimension ref="D6:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1816,7 @@
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="67" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1835,10 +1832,10 @@
         <f>G7*F7</f>
         <v>24120</v>
       </c>
-      <c r="I7" s="38"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="47"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1852,10 +1849,10 @@
         <f>G8*F8</f>
         <v>56760</v>
       </c>
-      <c r="I8" s="38"/>
+      <c r="I8" s="59"/>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="48"/>
+      <c r="D9" s="69"/>
       <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
@@ -1864,7 +1861,7 @@
       <c r="H9" s="2">
         <v>1000</v>
       </c>
-      <c r="I9" s="38"/>
+      <c r="I9" s="59"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10" s="9" t="s">
@@ -1880,10 +1877,10 @@
         <f>SUM(H7:H9)</f>
         <v>81880</v>
       </c>
-      <c r="I10" s="38"/>
+      <c r="I10" s="59"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1899,7 +1896,7 @@
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="44"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1911,7 +1908,7 @@
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="44"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1923,7 +1920,7 @@
       </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="45"/>
+      <c r="D14" s="66"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1977,7 +1974,7 @@
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="60" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="16">
@@ -1993,7 +1990,7 @@
       </c>
     </row>
     <row r="22" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="40"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="17">
         <v>660</v>
       </c>
@@ -2007,7 +2004,7 @@
       </c>
     </row>
     <row r="23" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="40"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="28" t="s">
         <v>10</v>
       </c>
@@ -2021,7 +2018,7 @@
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="62" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="16">
@@ -2036,7 +2033,7 @@
       </c>
     </row>
     <row r="25" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="41"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="17">
         <v>660</v>
       </c>
@@ -2049,7 +2046,7 @@
       </c>
     </row>
     <row r="26" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="42"/>
+      <c r="E26" s="63"/>
       <c r="F26" s="28" t="s">
         <v>10</v>
       </c>
@@ -2408,7 +2405,7 @@
       <c r="F7" s="2">
         <v>10000</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="59"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
@@ -2418,10 +2415,10 @@
       <c r="F8" s="9">
         <v>10000</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="59"/>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="70" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -2435,7 +2432,7 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="50"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="2" t="s">
         <v>63</v>
       </c>
@@ -2447,7 +2444,7 @@
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="51"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
@@ -2541,7 +2538,7 @@
       <c r="F7" s="2">
         <v>4000</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="59"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
@@ -2551,7 +2548,7 @@
       <c r="F8" s="9">
         <v>4000</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="59"/>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="11" t="s">
@@ -2612,7 +2609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977346C3-FB40-4906-BFEF-5578C3F0829E}">
   <dimension ref="D6:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2744,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA0FD11-AEA6-48EE-ACA9-F949F47C87AE}">
   <dimension ref="D5:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>